<commit_message>
test-17 (normpersoul, with popsize)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-17.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-17.xlsx
@@ -385,7 +385,7 @@
   <dimension ref="C3:Q57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V19" sqref="V19"/>
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,8 +457,12 @@
       <c r="O5" s="2">
         <v>1</v>
       </c>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
+      <c r="P5" s="3">
+        <v>40.853215315603983</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>108.9815951313261</v>
+      </c>
     </row>
     <row r="6" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
@@ -485,8 +489,12 @@
         <f>O5+1</f>
         <v>2</v>
       </c>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
+      <c r="P6" s="3">
+        <v>40.858750400512648</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>108.7688084561179</v>
+      </c>
     </row>
     <row r="7" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
@@ -513,8 +521,12 @@
         <f t="shared" ref="O7:O54" si="2">O6+1</f>
         <v>3</v>
       </c>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
+      <c r="P7" s="3">
+        <v>40.416924062800391</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>112.59673286354899</v>
+      </c>
     </row>
     <row r="8" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
@@ -541,8 +553,12 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
+      <c r="P8" s="3">
+        <v>41.036055751361737</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>109.3773030108905</v>
+      </c>
     </row>
     <row r="9" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
@@ -569,8 +585,12 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
+      <c r="P9" s="3">
+        <v>41.50213232938161</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>106.7052402306214</v>
+      </c>
     </row>
     <row r="10" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
@@ -597,8 +617,12 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
+      <c r="P10" s="3">
+        <v>40.308361102210831</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>112.2970916079436</v>
+      </c>
     </row>
     <row r="11" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
@@ -625,8 +649,12 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
+      <c r="P11" s="3">
+        <v>41.063115988465228</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>110.3929212043562</v>
+      </c>
     </row>
     <row r="12" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
@@ -653,8 +681,12 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
+      <c r="P12" s="3">
+        <v>40.275948413969878</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>113.6996540679052</v>
+      </c>
     </row>
     <row r="13" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
@@ -681,8 +713,12 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
+      <c r="P13" s="3">
+        <v>40.650972444729263</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>109.95288917360659</v>
+      </c>
     </row>
     <row r="14" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
@@ -709,8 +745,12 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
+      <c r="P14" s="3">
+        <v>40.502161166292851</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>109.67027546444589</v>
+      </c>
     </row>
     <row r="15" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
@@ -737,8 +777,12 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
+      <c r="P15" s="3">
+        <v>40.294458506888823</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>113.54431133888529</v>
+      </c>
     </row>
     <row r="16" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
@@ -765,8 +809,12 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
+      <c r="P16" s="3">
+        <v>41.283590195450167</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>105.5434913516976</v>
+      </c>
     </row>
     <row r="17" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
@@ -793,8 +841,12 @@
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
+      <c r="P17" s="3">
+        <v>41.262894905479023</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>107.3324727738629</v>
+      </c>
     </row>
     <row r="18" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
@@ -821,8 +873,12 @@
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
+      <c r="P18" s="3">
+        <v>40.386244793335479</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>113.72840486867391</v>
+      </c>
     </row>
     <row r="19" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
@@ -849,8 +905,12 @@
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
+      <c r="P19" s="3">
+        <v>41.072569689202183</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>106.89323510570151</v>
+      </c>
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
@@ -877,8 +937,12 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
+      <c r="P20" s="3">
+        <v>41.060696892021788</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>107.0167392696989</v>
+      </c>
     </row>
     <row r="21" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
@@ -905,8 +969,12 @@
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
+      <c r="P21" s="3">
+        <v>40.798438000640807</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>108.9946828955797</v>
+      </c>
     </row>
     <row r="22" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
@@ -933,8 +1001,12 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
+      <c r="P22" s="3">
+        <v>40.544508170458187</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>105.9071748878924</v>
+      </c>
     </row>
     <row r="23" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
@@ -961,8 +1033,12 @@
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
+      <c r="P23" s="3">
+        <v>40.692947773149619</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>113.0381550288277</v>
+      </c>
     </row>
     <row r="24" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
@@ -989,8 +1065,12 @@
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
+      <c r="P24" s="3">
+        <v>40.733973085549501</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>109.75424087123641</v>
+      </c>
     </row>
     <row r="25" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
@@ -1017,8 +1097,12 @@
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
+      <c r="P25" s="3">
+        <v>41.173715155398909</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>106.21046764894299</v>
+      </c>
     </row>
     <row r="26" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
@@ -1045,8 +1129,12 @@
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
+      <c r="P26" s="3">
+        <v>40.838711951297661</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>107.90310698270341</v>
+      </c>
     </row>
     <row r="27" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
@@ -1073,8 +1161,12 @@
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="3"/>
+      <c r="P27" s="3">
+        <v>40.936094200576733</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>106.2937411915439</v>
+      </c>
     </row>
     <row r="28" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
@@ -1101,8 +1193,12 @@
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
+      <c r="P28" s="3">
+        <v>41.332866068567768</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>105.5442921204356</v>
+      </c>
     </row>
     <row r="29" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
@@ -1129,8 +1225,12 @@
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
+      <c r="P29" s="3">
+        <v>40.827835629605893</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>107.0605637411916</v>
+      </c>
     </row>
     <row r="30" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
@@ -1157,8 +1257,12 @@
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
+      <c r="P30" s="3">
+        <v>40.839778917013767</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>105.99584240871241</v>
+      </c>
     </row>
     <row r="31" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
@@ -1185,8 +1289,12 @@
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
+      <c r="P31" s="3">
+        <v>40.723522909323933</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>106.153196668802</v>
+      </c>
     </row>
     <row r="32" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
@@ -1213,8 +1321,12 @@
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="3"/>
+      <c r="P32" s="3">
+        <v>41.11888176866389</v>
+      </c>
+      <c r="Q32" s="3">
+        <v>105.5787700192185</v>
+      </c>
     </row>
     <row r="33" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
@@ -1241,8 +1353,12 @@
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="P33" s="3"/>
-      <c r="Q33" s="3"/>
+      <c r="P33" s="3">
+        <v>41.073886574815774</v>
+      </c>
+      <c r="Q33" s="3">
+        <v>109.36764253683531</v>
+      </c>
     </row>
     <row r="34" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
@@ -1269,8 +1385,12 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="P34" s="3"/>
-      <c r="Q34" s="3"/>
+      <c r="P34" s="3">
+        <v>40.840341236783082</v>
+      </c>
+      <c r="Q34" s="3">
+        <v>110.2749775784753</v>
+      </c>
     </row>
     <row r="35" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
@@ -1297,8 +1417,12 @@
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="P35" s="3"/>
-      <c r="Q35" s="3"/>
+      <c r="P35" s="3">
+        <v>40.353617430310798</v>
+      </c>
+      <c r="Q35" s="3">
+        <v>116.54948110185779</v>
+      </c>
     </row>
     <row r="36" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
@@ -1325,8 +1449,12 @@
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="P36" s="3"/>
-      <c r="Q36" s="3"/>
+      <c r="P36" s="3">
+        <v>40.660355655238703</v>
+      </c>
+      <c r="Q36" s="3">
+        <v>112.5405509288917</v>
+      </c>
     </row>
     <row r="37" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
@@ -1353,8 +1481,12 @@
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="P37" s="3"/>
-      <c r="Q37" s="3"/>
+      <c r="P37" s="3">
+        <v>40.65428548542134</v>
+      </c>
+      <c r="Q37" s="3">
+        <v>112.14438821268411</v>
+      </c>
     </row>
     <row r="38" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
@@ -1381,8 +1513,12 @@
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3"/>
+      <c r="P38" s="3">
+        <v>41.107518423582178</v>
+      </c>
+      <c r="Q38" s="3">
+        <v>106.7093914157591</v>
+      </c>
     </row>
     <row r="39" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
@@ -1409,8 +1545,12 @@
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
+      <c r="P39" s="3">
+        <v>41.073112784363992</v>
+      </c>
+      <c r="Q39" s="3">
+        <v>108.79917360666239</v>
+      </c>
     </row>
     <row r="40" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
@@ -1437,8 +1577,12 @@
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="P40" s="3"/>
-      <c r="Q40" s="3"/>
+      <c r="P40" s="3">
+        <v>40.658123998718359</v>
+      </c>
+      <c r="Q40" s="3">
+        <v>109.6595259449071</v>
+      </c>
     </row>
     <row r="41" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
@@ -1465,8 +1609,12 @@
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="P41" s="3"/>
-      <c r="Q41" s="3"/>
+      <c r="P41" s="3">
+        <v>40.1263889778917</v>
+      </c>
+      <c r="Q41" s="3">
+        <v>113.15373478539399</v>
+      </c>
     </row>
     <row r="42" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
@@ -1493,8 +1641,12 @@
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="P42" s="3"/>
-      <c r="Q42" s="3"/>
+      <c r="P42" s="3">
+        <v>41.293018263377121</v>
+      </c>
+      <c r="Q42" s="3">
+        <v>104.747732222934</v>
+      </c>
     </row>
     <row r="43" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
@@ -1521,8 +1673,12 @@
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="P43" s="3"/>
-      <c r="Q43" s="3"/>
+      <c r="P43" s="3">
+        <v>41.497281320089719</v>
+      </c>
+      <c r="Q43" s="3">
+        <v>104.9949199231262</v>
+      </c>
     </row>
     <row r="44" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
@@ -1549,8 +1705,12 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="P44" s="3"/>
-      <c r="Q44" s="3"/>
+      <c r="P44" s="3">
+        <v>41.45328580583147</v>
+      </c>
+      <c r="Q44" s="3">
+        <v>104.20614349775779</v>
+      </c>
     </row>
     <row r="45" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
@@ -1577,8 +1737,12 @@
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="P45" s="3"/>
-      <c r="Q45" s="3"/>
+      <c r="P45" s="3">
+        <v>41.141738224927913</v>
+      </c>
+      <c r="Q45" s="3">
+        <v>105.4260794362588</v>
+      </c>
     </row>
     <row r="46" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
@@ -1605,8 +1769,12 @@
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="P46" s="3"/>
-      <c r="Q46" s="3"/>
+      <c r="P46" s="3">
+        <v>40.202502403075933</v>
+      </c>
+      <c r="Q46" s="3">
+        <v>112.0481934657271</v>
+      </c>
     </row>
     <row r="47" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
@@ -1633,8 +1801,12 @@
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="P47" s="3"/>
-      <c r="Q47" s="3"/>
+      <c r="P47" s="3">
+        <v>40.088466837552062</v>
+      </c>
+      <c r="Q47" s="3">
+        <v>117.9945868033312</v>
+      </c>
     </row>
     <row r="48" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
@@ -1661,8 +1833,12 @@
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="P48" s="3"/>
-      <c r="Q48" s="3"/>
+      <c r="P48" s="3">
+        <v>40.652596924062799</v>
+      </c>
+      <c r="Q48" s="3">
+        <v>112.2269506726457</v>
+      </c>
     </row>
     <row r="49" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
@@ -1689,8 +1865,12 @@
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="P49" s="3"/>
-      <c r="Q49" s="3"/>
+      <c r="P49" s="3">
+        <v>40.406108619032359</v>
+      </c>
+      <c r="Q49" s="3">
+        <v>112.9717937219731</v>
+      </c>
     </row>
     <row r="50" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
@@ -1717,8 +1897,12 @@
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="P50" s="3"/>
-      <c r="Q50" s="3"/>
+      <c r="P50" s="3">
+        <v>41.150791413008641</v>
+      </c>
+      <c r="Q50" s="3">
+        <v>107.4082190903267</v>
+      </c>
     </row>
     <row r="51" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
@@ -1745,8 +1929,12 @@
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="P51" s="3"/>
-      <c r="Q51" s="3"/>
+      <c r="P51" s="3">
+        <v>40.924032361422618</v>
+      </c>
+      <c r="Q51" s="3">
+        <v>106.4392568866111</v>
+      </c>
     </row>
     <row r="52" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
@@ -1773,8 +1961,12 @@
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="P52" s="3"/>
-      <c r="Q52" s="3"/>
+      <c r="P52" s="3">
+        <v>41.073474847805187</v>
+      </c>
+      <c r="Q52" s="3">
+        <v>104.46516976297239</v>
+      </c>
     </row>
     <row r="53" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
@@ -1801,8 +1993,12 @@
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="P53" s="3"/>
-      <c r="Q53" s="3"/>
+      <c r="P53" s="3">
+        <v>40.657516821531559</v>
+      </c>
+      <c r="Q53" s="3">
+        <v>112.5238565022422</v>
+      </c>
     </row>
     <row r="54" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
@@ -1829,8 +2025,12 @@
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="P54" s="3"/>
-      <c r="Q54" s="3"/>
+      <c r="P54" s="3">
+        <v>40.820836270426142</v>
+      </c>
+      <c r="Q54" s="3">
+        <v>110.7881165919282</v>
+      </c>
     </row>
     <row r="56" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
@@ -1858,13 +2058,13 @@
       <c r="O56" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P56" s="3" t="e">
+      <c r="P56" s="3">
         <f>AVERAGE(P5:P54)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q56" s="3" t="e">
+        <v>40.825972925344438</v>
+      </c>
+      <c r="Q56" s="3">
         <f>AVERAGE(Q5:Q54)</f>
-        <v>#DIV/0!</v>
+        <v>109.20750570147342</v>
       </c>
     </row>
     <row r="57" spans="3:17" x14ac:dyDescent="0.25">
@@ -1893,13 +2093,13 @@
       <c r="O57" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P57" s="3" t="e">
+      <c r="P57" s="3">
         <f>_xlfn.STDEV.S(P5:P54)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q57" s="3" t="e">
+        <v>0.36485675971433584</v>
+      </c>
+      <c r="Q57" s="3">
         <f>_xlfn.STDEV.S(Q5:Q54)</f>
-        <v>#DIV/0!</v>
+        <v>3.3245518899473501</v>
       </c>
     </row>
   </sheetData>

</xml_diff>